<commit_message>
move the bremer/dennis file to the right place
</commit_message>
<xml_diff>
--- a/data/physiology/coli_metabolic_modes.xlsx
+++ b/data/physiology/coli_metabolic_modes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flamholz/Documents/workspace/redox-proteome/data/physiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999CE344-C78F-6F42-9FDC-105A4995EC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CC4752-D6FF-CB4F-82C2-F2542A0400BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30100" yWindow="1040" windowWidth="26840" windowHeight="15440" xr2:uid="{0292FDAA-60A7-F643-98AE-4ABDDCCE6051}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{0292FDAA-60A7-F643-98AE-4ABDDCCE6051}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>amino acids</t>
   </si>
@@ -53,9 +53,6 @@
     <t>fermentation</t>
   </si>
   <si>
-    <t>CO2</t>
-  </si>
-  <si>
     <t>sugars</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
   </si>
   <si>
     <t>model</t>
-  </si>
-  <si>
-    <t>formate</t>
-  </si>
-  <si>
-    <t>engineered</t>
   </si>
   <si>
     <t>e_donor</t>
@@ -435,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C8E46A-3B3C-484D-8E36-CE8819AECA49}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,9 +438,9 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -463,100 +454,89 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>